<commit_message>
fixed. telecoms-japan and type "Departiment" to Department
</commit_message>
<xml_diff>
--- a/mapping/mml_referral_mapping.xlsx
+++ b/mapping/mml_referral_mapping.xlsx
@@ -986,26 +986,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Departiment']/items[at0001]/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Departiment']/items[at0.15]/defining_code/code_string</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Departiment']/items[at0.15]/defining_code/terminology_id/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Departiment']/items[at0011.1]/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Departiment']/items[at0.12]/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>DV_IDENTIFIER</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1014,10 +994,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Departiment']/items[at0.13]/magnitude</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>DV_CODED_TEXT</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1058,10 +1034,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Departiment']/items[at0.14]/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.address-japan.v1 and name/value='Address expression of Japan']/items[at0001 and name/value='Address']/items[at0002]/value</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1082,42 +1054,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.telecom_details-mml.v1 and name/value='Telecom details for MML']/items[at0009 and name/value='Email address']/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.telecom_details-mml.v1 and name/value='Telecom details for MML']/items[at0001 and name/value='Telecoms']/items[at0002.1]/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.telecom_details-mml.v1 and name/value='Telecom details for MML']/items[at0001 and name/value='Telecoms']/items[at0003]/items[at0006]/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.telecom_details-mml.v1 and name/value='Telecom details for MML']/items[at0001 and name/value='Telecoms']/items[at0003]/items[at0.21]/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.telecom_details-mml.v1 and name/value='Telecom details for MML']/items[at0001 and name/value='Telecoms']/items[at0003]/items[at0007]/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.telecom_details-mml.v1 and name/value='Telecom details for MML']/items[at0001 and name/value='Telecoms']/items[at0003]/items[at0019]/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.telecom_details-mml.v1 and name/value='Telecom details for MML']/items[at0001 and name/value='Telecoms']/items[at0003]/items[at0005]/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.telecom_details-mml.v1 and name/value='Telecom details for MML']/items[at0.20]/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.telecom_details-mml.v1 and name/value='Telecom details for MML']/items[at0001 and name/value='Telecoms']/items[at0004]/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/activities[at0001 and name/value='Request']/description[at0009]/items[at0121]/value</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1534,10 +1470,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Departiment']/items[at0.12]/mappings/match</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='refer to facility']/items[at0.12]/mappings/match/defining_code/terminology_id/value</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1570,10 +1502,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Departiment']/items[at0.12]/mappings/target/defining_code/terminology_id/value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>master id/checkDigitSchema</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1678,6 +1606,61 @@
   <si>
     <t>1.10.1.</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.telecom_details-japan.v1 and name/value='Telecom details for MML']/items[at0009 and name/value='Email address']/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.telecom_details-japan.v1 and name/value='Telecom details for MML']/items[at0001 and name/value='Telecoms']/items[at0004]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.telecom_details-japan.v1 and name/value='Telecom details for MML']/items[at0001 and name/value='Telecoms']/items[at0003]/items[at0006]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.telecom_details-japan.v1 and name/value='Telecom details for MML']/items[at0001 and name/value='Telecoms']/items[at0003]/items[at0.21]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.telecom_details-japan.v1 and name/value='Telecom details for MML']/items[at0001 and name/value='Telecoms']/items[at0003]/items[at0007]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.telecom_details-japan.v1 and name/value='Telecom details for MML']/items[at0001 and name/value='Telecoms']/items[at0003]/items[at0019]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.telecom_details-japan.v1 and name/value='Telecom details for MML']/items[at0001 and name/value='Telecoms']/items[at0002.1]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.telecom_details-japan.v1 and name/value='Telecom details for MML']/items[at0001 and name/value='Telecoms']/items[at0003]/items[at0005]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.telecom_details-japan.v1 and name/value='Telecom details for MML']/items[at0.20]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Department']/items[at0001]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Department']/items[at0.15]/defining_code/code_string</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Department']/items[at0.15]/defining_code/terminology_id/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Department']/items[at0011.1]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Department']/items[at0.12]/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Department']/items[at0.12]/mappings/target/defining_code/terminology_id/value</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Department']/items[at0.12]/mappings/match</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Department']/items[at0.13]/magnitude</t>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.referral_details.v1 and name/value='Referral Details']/items[openEHR-EHR-INSTRUCTION.request-referral.v1]/protocol[at0008]/items[openEHR-EHR-CLUSTER.individual_professional-mml.v1 and name/value='refer from person']/items[at0003]/items[openEHR-EHR-CLUSTER.organisation-mml.v1 and name/value='Department']/items[at0.14]/value</t>
   </si>
 </sst>
 </file>
@@ -2182,8 +2165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A212" workbookViewId="0">
-      <selection activeCell="H207" sqref="H207"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="K97" sqref="K97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2199,7 +2182,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>423</v>
+        <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
@@ -2405,7 +2388,7 @@
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="22" t="s">
-        <v>414</v>
+        <v>396</v>
       </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
@@ -2830,7 +2813,7 @@
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
       <c r="I33" s="23" t="s">
-        <v>424</v>
+        <v>406</v>
       </c>
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
@@ -3004,7 +2987,7 @@
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
       <c r="I41" s="23" t="s">
-        <v>415</v>
+        <v>397</v>
       </c>
       <c r="J41" s="17"/>
       <c r="K41" s="7"/>
@@ -3270,7 +3253,7 @@
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
       <c r="I54" s="23" t="s">
-        <v>425</v>
+        <v>407</v>
       </c>
       <c r="J54" s="12"/>
       <c r="K54" s="7"/>
@@ -3313,7 +3296,7 @@
       <c r="G56" s="9"/>
       <c r="H56" s="9"/>
       <c r="I56" s="23" t="s">
-        <v>426</v>
+        <v>408</v>
       </c>
       <c r="J56" s="16"/>
       <c r="K56" s="7"/>
@@ -3356,7 +3339,7 @@
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
       <c r="I58" s="23" t="s">
-        <v>427</v>
+        <v>409</v>
       </c>
       <c r="K58" s="7"/>
       <c r="L58" s="7"/>
@@ -3510,7 +3493,7 @@
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
       <c r="I65" s="25" t="s">
-        <v>428</v>
+        <v>410</v>
       </c>
       <c r="J65" s="14"/>
       <c r="K65" s="7"/>
@@ -3585,7 +3568,7 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A69" s="3" t="s">
-        <v>430</v>
+        <v>412</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>180</v>
@@ -3660,7 +3643,7 @@
       </c>
       <c r="F72" s="3"/>
       <c r="K72" s="7" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
       <c r="L72" s="7"/>
     </row>
@@ -3675,7 +3658,7 @@
         <v>262</v>
       </c>
       <c r="K73" s="7" t="s">
-        <v>401</v>
+        <v>385</v>
       </c>
       <c r="L73" s="7"/>
     </row>
@@ -3699,7 +3682,7 @@
         <v>243</v>
       </c>
       <c r="K74" s="7" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="L74" s="7"/>
     </row>
@@ -3723,7 +3706,7 @@
         <v>245</v>
       </c>
       <c r="K75" s="7" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="L75" s="7"/>
     </row>
@@ -3969,7 +3952,7 @@
       </c>
       <c r="F87" s="3"/>
       <c r="I87" s="24" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="J87" s="12" t="s">
         <v>255</v>
@@ -4087,7 +4070,7 @@
       </c>
       <c r="F92" s="3"/>
       <c r="K92" s="7" t="s">
-        <v>402</v>
+        <v>386</v>
       </c>
       <c r="L92" s="7"/>
     </row>
@@ -4101,7 +4084,7 @@
         <v>262</v>
       </c>
       <c r="K93" s="7" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
       <c r="L93" s="7"/>
     </row>
@@ -4143,7 +4126,7 @@
         <v>24</v>
       </c>
       <c r="I95" s="24" t="s">
-        <v>417</v>
+        <v>399</v>
       </c>
       <c r="J95" s="12" t="s">
         <v>255</v>
@@ -4182,13 +4165,13 @@
       </c>
       <c r="F97" s="3"/>
       <c r="I97" s="24" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="J97" s="13" t="s">
         <v>255</v>
       </c>
       <c r="K97" s="12" t="s">
-        <v>267</v>
+        <v>432</v>
       </c>
       <c r="L97" s="7"/>
     </row>
@@ -4214,7 +4197,7 @@
         <v>257</v>
       </c>
       <c r="K98" s="12" t="s">
-        <v>268</v>
+        <v>433</v>
       </c>
       <c r="L98" s="7"/>
     </row>
@@ -4233,7 +4216,7 @@
       <c r="F99" s="3"/>
       <c r="I99" s="18"/>
       <c r="K99" s="12" t="s">
-        <v>269</v>
+        <v>434</v>
       </c>
       <c r="L99" s="7"/>
     </row>
@@ -4254,10 +4237,10 @@
         <v>184</v>
       </c>
       <c r="J100" s="13" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="K100" s="12" t="s">
-        <v>270</v>
+        <v>435</v>
       </c>
       <c r="L100" s="7"/>
     </row>
@@ -4282,7 +4265,7 @@
         <v>255</v>
       </c>
       <c r="K101" s="12" t="s">
-        <v>271</v>
+        <v>436</v>
       </c>
       <c r="L101" s="7"/>
     </row>
@@ -4299,7 +4282,7 @@
       </c>
       <c r="F102" s="3"/>
       <c r="K102" s="12" t="s">
-        <v>413</v>
+        <v>437</v>
       </c>
       <c r="L102" s="7"/>
     </row>
@@ -4313,7 +4296,7 @@
         <v>262</v>
       </c>
       <c r="K103" s="12" t="s">
-        <v>404</v>
+        <v>438</v>
       </c>
       <c r="L103" s="7"/>
     </row>
@@ -4333,10 +4316,10 @@
         <v>186</v>
       </c>
       <c r="J104" s="12" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="K104" s="7" t="s">
-        <v>274</v>
+        <v>439</v>
       </c>
       <c r="L104" s="7"/>
     </row>
@@ -4355,13 +4338,13 @@
         <v>24</v>
       </c>
       <c r="I105" s="24" t="s">
-        <v>417</v>
+        <v>399</v>
       </c>
       <c r="J105" s="12" t="s">
         <v>255</v>
       </c>
       <c r="K105" s="7" t="s">
-        <v>285</v>
+        <v>440</v>
       </c>
       <c r="L105" s="7"/>
     </row>
@@ -4417,10 +4400,10 @@
         <v>153</v>
       </c>
       <c r="J108" s="17" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="K108" s="7" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="L108" s="7"/>
     </row>
@@ -4440,13 +4423,13 @@
         <v>44</v>
       </c>
       <c r="I109" s="25" t="s">
-        <v>415</v>
+        <v>397</v>
       </c>
       <c r="J109" s="17" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="K109" s="7" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="L109" s="7"/>
     </row>
@@ -4466,7 +4449,7 @@
       <c r="I110" s="17"/>
       <c r="J110" s="17"/>
       <c r="K110" s="7" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="L110" s="7"/>
     </row>
@@ -4487,10 +4470,10 @@
         <v>154</v>
       </c>
       <c r="J111" s="13" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="K111" s="7" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="L111" s="7"/>
     </row>
@@ -4514,7 +4497,7 @@
         <v>255</v>
       </c>
       <c r="K112" s="7" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="L112" s="7"/>
     </row>
@@ -4538,7 +4521,7 @@
         <v>255</v>
       </c>
       <c r="K113" s="7" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="L113" s="7"/>
     </row>
@@ -4562,7 +4545,7 @@
         <v>255</v>
       </c>
       <c r="K114" s="7" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="L114" s="7"/>
     </row>
@@ -4586,7 +4569,7 @@
         <v>255</v>
       </c>
       <c r="K115" s="7" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="L115" s="7"/>
     </row>
@@ -4610,7 +4593,7 @@
         <v>255</v>
       </c>
       <c r="K116" s="7" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="L116" s="7"/>
     </row>
@@ -4634,7 +4617,7 @@
         <v>255</v>
       </c>
       <c r="K117" s="7" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="L117" s="7"/>
     </row>
@@ -4675,7 +4658,7 @@
         <v>255</v>
       </c>
       <c r="K119" s="7" t="s">
-        <v>291</v>
+        <v>423</v>
       </c>
       <c r="L119" s="7"/>
     </row>
@@ -4726,13 +4709,13 @@
         <v>59</v>
       </c>
       <c r="I122" s="25" t="s">
-        <v>425</v>
+        <v>407</v>
       </c>
       <c r="J122" s="12" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="K122" s="7" t="s">
-        <v>299</v>
+        <v>424</v>
       </c>
       <c r="L122" s="7"/>
     </row>
@@ -4753,10 +4736,10 @@
         <v>199</v>
       </c>
       <c r="J123" s="13" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="K123" s="7" t="s">
-        <v>293</v>
+        <v>425</v>
       </c>
       <c r="L123" s="7"/>
     </row>
@@ -4774,13 +4757,13 @@
       </c>
       <c r="F124" s="3"/>
       <c r="I124" s="23" t="s">
-        <v>426</v>
+        <v>408</v>
       </c>
       <c r="J124" s="16" t="s">
         <v>255</v>
       </c>
       <c r="K124" s="7" t="s">
-        <v>294</v>
+        <v>426</v>
       </c>
       <c r="L124" s="7"/>
     </row>
@@ -4804,7 +4787,7 @@
         <v>255</v>
       </c>
       <c r="K125" s="7" t="s">
-        <v>295</v>
+        <v>427</v>
       </c>
       <c r="L125" s="7"/>
     </row>
@@ -4822,13 +4805,13 @@
       </c>
       <c r="F126" s="3"/>
       <c r="I126" s="25" t="s">
-        <v>429</v>
+        <v>411</v>
       </c>
       <c r="J126" s="13" t="s">
         <v>255</v>
       </c>
       <c r="K126" s="7" t="s">
-        <v>296</v>
+        <v>428</v>
       </c>
       <c r="L126" s="7"/>
     </row>
@@ -4852,7 +4835,7 @@
         <v>255</v>
       </c>
       <c r="K127" s="7" t="s">
-        <v>292</v>
+        <v>429</v>
       </c>
       <c r="L127" s="7"/>
     </row>
@@ -4876,7 +4859,7 @@
         <v>255</v>
       </c>
       <c r="K128" s="7" t="s">
-        <v>297</v>
+        <v>430</v>
       </c>
       <c r="L128" s="7"/>
     </row>
@@ -4900,13 +4883,13 @@
         <v>255</v>
       </c>
       <c r="K129" s="7" t="s">
-        <v>298</v>
+        <v>431</v>
       </c>
       <c r="L129" s="7"/>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A130" s="3" t="s">
-        <v>431</v>
+        <v>413</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>74</v>
@@ -4927,13 +4910,13 @@
         <v>255</v>
       </c>
       <c r="K130" s="7" t="s">
-        <v>300</v>
+        <v>284</v>
       </c>
       <c r="L130" s="7"/>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A131" s="3" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>75</v>
@@ -4948,19 +4931,19 @@
       <c r="F131" s="3"/>
       <c r="H131" s="7"/>
       <c r="I131" s="12" t="s">
-        <v>301</v>
+        <v>285</v>
       </c>
       <c r="J131" s="12" t="s">
         <v>255</v>
       </c>
       <c r="K131" s="7" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
       <c r="L131" s="7"/>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A132" s="3" t="s">
-        <v>433</v>
+        <v>415</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>76</v>
@@ -4981,13 +4964,13 @@
         <v>255</v>
       </c>
       <c r="K132" s="7" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="L132" s="7"/>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A133" s="3" t="s">
-        <v>434</v>
+        <v>416</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>77</v>
@@ -5004,19 +4987,19 @@
         <v>207</v>
       </c>
       <c r="I133" s="12" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
       <c r="J133" s="12" t="s">
         <v>255</v>
       </c>
       <c r="K133" s="7" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
       <c r="L133" s="7"/>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A134" s="3" t="s">
-        <v>435</v>
+        <v>417</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>78</v>
@@ -5039,13 +5022,13 @@
         <v>255</v>
       </c>
       <c r="K134" s="7" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="L134" s="7"/>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A135" s="3" t="s">
-        <v>436</v>
+        <v>418</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>16</v>
@@ -5057,7 +5040,7 @@
       </c>
       <c r="F135" s="3"/>
       <c r="H135" s="7" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="L135" s="7"/>
     </row>
@@ -5065,28 +5048,28 @@
       <c r="A136" s="3"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="E136" s="3"/>
       <c r="F136" s="3"/>
       <c r="H136" s="7"/>
       <c r="I136" s="12" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="J136" s="12" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="K136" s="7" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="L136" s="7"/>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A137" s="3" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>79</v>
@@ -5109,13 +5092,13 @@
         <v>255</v>
       </c>
       <c r="K137" s="7" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="L137" s="7"/>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A138" s="3" t="s">
-        <v>438</v>
+        <v>420</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>16</v>
@@ -5138,26 +5121,26 @@
       <c r="A139" s="3"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="D139" s="3"/>
       <c r="E139" s="3"/>
       <c r="F139" s="3"/>
       <c r="H139" s="7"/>
       <c r="I139" s="12" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="J139" s="12" t="s">
         <v>255</v>
       </c>
       <c r="K139" s="7" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="L139" s="7"/>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A140" s="3" t="s">
-        <v>439</v>
+        <v>421</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>80</v>
@@ -5175,16 +5158,16 @@
         <v>213</v>
       </c>
       <c r="J140" s="12" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="K140" s="7" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="L140" s="7"/>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A141" s="3" t="s">
-        <v>440</v>
+        <v>422</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>16</v>
@@ -5196,7 +5179,7 @@
       </c>
       <c r="F141" s="3"/>
       <c r="H141" s="7" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="K141" s="7"/>
       <c r="L141" s="7"/>
@@ -5205,20 +5188,20 @@
       <c r="A142" s="3"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="D142" s="3"/>
       <c r="E142" s="3"/>
       <c r="F142" s="3"/>
       <c r="H142" s="7"/>
       <c r="I142" s="12" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="J142" s="12" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="K142" s="7" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="L142" s="7"/>
     </row>
@@ -5238,16 +5221,16 @@
       </c>
       <c r="F143" s="3"/>
       <c r="H143" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="I143" s="12" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="J143" s="12" t="s">
         <v>255</v>
       </c>
       <c r="K143" s="7" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="L143" s="7"/>
     </row>
@@ -5265,7 +5248,7 @@
       </c>
       <c r="F144" s="3"/>
       <c r="H144" s="7" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="I144" s="12"/>
       <c r="J144" s="12"/>
@@ -5276,21 +5259,21 @@
       <c r="A145" s="3"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="E145" s="3"/>
       <c r="F145" s="3"/>
       <c r="I145" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="J145" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="K145" s="7" t="s">
         <v>308</v>
-      </c>
-      <c r="J145" s="12" t="s">
-        <v>309</v>
-      </c>
-      <c r="K145" s="7" t="s">
-        <v>324</v>
       </c>
       <c r="L145" s="7"/>
     </row>
@@ -5317,7 +5300,7 @@
         <v>255</v>
       </c>
       <c r="K146" s="7" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="L146" s="7"/>
     </row>
@@ -5337,16 +5320,16 @@
       </c>
       <c r="F147" s="3"/>
       <c r="H147" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="I147" s="12" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="J147" s="12" t="s">
         <v>255</v>
       </c>
       <c r="K147" s="7" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="L147" s="7"/>
     </row>
@@ -5375,19 +5358,19 @@
       <c r="A149" s="3"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="D149" s="3"/>
       <c r="E149" s="3"/>
       <c r="F149" s="3"/>
       <c r="I149" s="12" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="J149" s="12" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="K149" s="7" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="L149" s="7"/>
     </row>
@@ -5414,7 +5397,7 @@
         <v>255</v>
       </c>
       <c r="K150" s="7" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="L150" s="7"/>
     </row>
@@ -5440,10 +5423,10 @@
         <v>219</v>
       </c>
       <c r="J151" s="12" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="K151" s="7" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="L151" s="7"/>
     </row>
@@ -5472,19 +5455,19 @@
       <c r="A153" s="3"/>
       <c r="B153" s="3"/>
       <c r="C153" s="3" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="D153" s="3"/>
       <c r="E153" s="3"/>
       <c r="F153" s="3"/>
       <c r="I153" s="12" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="J153" s="12" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="K153" s="27" t="s">
-        <v>422</v>
+        <v>404</v>
       </c>
       <c r="L153" s="7"/>
     </row>
@@ -5502,7 +5485,7 @@
       <c r="I154" s="12"/>
       <c r="J154" s="12"/>
       <c r="K154" s="7" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="L154" s="7"/>
     </row>
@@ -5538,13 +5521,13 @@
       </c>
       <c r="F156" s="3"/>
       <c r="I156" s="24" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="J156" s="12" t="s">
         <v>255</v>
       </c>
       <c r="K156" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="L156" s="7"/>
     </row>
@@ -5567,10 +5550,10 @@
         <v>125</v>
       </c>
       <c r="J157" s="12" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="K157" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="L157" s="7"/>
     </row>
@@ -5590,7 +5573,7 @@
       <c r="I158" s="18"/>
       <c r="J158" s="18"/>
       <c r="K158" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
       <c r="L158" s="7"/>
     </row>
@@ -5611,10 +5594,10 @@
         <v>184</v>
       </c>
       <c r="J159" s="12" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="K159" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="L159" s="7"/>
     </row>
@@ -5639,7 +5622,7 @@
         <v>255</v>
       </c>
       <c r="K160" s="27" t="s">
-        <v>421</v>
+        <v>403</v>
       </c>
       <c r="L160" s="7"/>
     </row>
@@ -5656,7 +5639,7 @@
       </c>
       <c r="F161" s="3"/>
       <c r="K161" t="s">
-        <v>405</v>
+        <v>388</v>
       </c>
       <c r="L161" s="7"/>
     </row>
@@ -5670,7 +5653,7 @@
         <v>262</v>
       </c>
       <c r="K162" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="L162" s="7"/>
     </row>
@@ -5693,7 +5676,7 @@
         <v>264</v>
       </c>
       <c r="K163" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="L163" s="7"/>
     </row>
@@ -5712,13 +5695,13 @@
         <v>24</v>
       </c>
       <c r="I164" s="24" t="s">
-        <v>417</v>
+        <v>399</v>
       </c>
       <c r="J164" s="12" t="s">
         <v>255</v>
       </c>
       <c r="K164" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="L164" s="7"/>
     </row>
@@ -5752,13 +5735,13 @@
       </c>
       <c r="F166" s="3"/>
       <c r="I166" s="24" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="J166" s="12" t="s">
         <v>255</v>
       </c>
       <c r="K166" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="L166" s="7"/>
     </row>
@@ -5781,10 +5764,10 @@
         <v>125</v>
       </c>
       <c r="J167" s="12" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="K167" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="L167" s="7"/>
     </row>
@@ -5804,7 +5787,7 @@
       <c r="I168" s="18"/>
       <c r="J168" s="18"/>
       <c r="K168" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="L168" s="7"/>
     </row>
@@ -5825,10 +5808,10 @@
         <v>184</v>
       </c>
       <c r="J169" s="12" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="K169" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="L169" s="7"/>
     </row>
@@ -5850,10 +5833,10 @@
         <v>185</v>
       </c>
       <c r="J170" s="12" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="K170" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="L170" s="7"/>
     </row>
@@ -5870,7 +5853,7 @@
       </c>
       <c r="F171" s="3"/>
       <c r="K171" t="s">
-        <v>407</v>
+        <v>390</v>
       </c>
       <c r="L171" s="7"/>
     </row>
@@ -5884,7 +5867,7 @@
         <v>262</v>
       </c>
       <c r="K172" t="s">
-        <v>408</v>
+        <v>391</v>
       </c>
       <c r="L172" s="7"/>
     </row>
@@ -5907,7 +5890,7 @@
         <v>264</v>
       </c>
       <c r="K173" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="L173" s="7"/>
     </row>
@@ -5926,13 +5909,13 @@
         <v>24</v>
       </c>
       <c r="I174" s="24" t="s">
-        <v>417</v>
+        <v>399</v>
       </c>
       <c r="J174" s="12" t="s">
         <v>255</v>
       </c>
       <c r="K174" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="L174" s="7"/>
     </row>
@@ -5967,7 +5950,7 @@
       <c r="E176" s="3"/>
       <c r="F176" s="3"/>
       <c r="H176" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="K176" s="7"/>
       <c r="L176" s="7"/>
@@ -5984,13 +5967,13 @@
       <c r="E177" s="3"/>
       <c r="F177" s="3"/>
       <c r="I177" s="13" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
       <c r="J177" s="13" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="K177" s="7" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="L177" s="7"/>
     </row>
@@ -6008,13 +5991,13 @@
       </c>
       <c r="F178" s="3"/>
       <c r="I178" s="13" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
       <c r="J178" s="13" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="K178" s="7" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
       <c r="L178" s="7"/>
     </row>
@@ -6032,7 +6015,7 @@
       </c>
       <c r="F179" s="3"/>
       <c r="K179" s="7" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
       <c r="L179" s="7"/>
     </row>
@@ -6047,7 +6030,7 @@
         <v>262</v>
       </c>
       <c r="K180" s="7" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="L180" s="7"/>
     </row>
@@ -6071,7 +6054,7 @@
         <v>264</v>
       </c>
       <c r="K181" s="7" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="L181" s="7"/>
     </row>
@@ -6095,7 +6078,7 @@
         <v>255</v>
       </c>
       <c r="K182" s="7" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="L182" s="7"/>
     </row>
@@ -6147,10 +6130,10 @@
         <v>125</v>
       </c>
       <c r="J185" s="15" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="K185" s="7" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
       <c r="L185" s="7"/>
     </row>
@@ -6168,7 +6151,7 @@
       </c>
       <c r="F186" s="3"/>
       <c r="K186" s="7" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="L186" s="7"/>
     </row>
@@ -6187,10 +6170,10 @@
         <v>126</v>
       </c>
       <c r="J187" s="12" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="K187" s="7" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
       <c r="L187" s="7"/>
     </row>
@@ -6212,7 +6195,7 @@
         <v>255</v>
       </c>
       <c r="K188" s="7" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="L188" s="7"/>
     </row>
@@ -6236,7 +6219,7 @@
         <v>255</v>
       </c>
       <c r="K189" s="7" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="L189" s="7"/>
     </row>
@@ -6258,7 +6241,7 @@
         <v>255</v>
       </c>
       <c r="K190" s="7" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="L190" s="7"/>
     </row>
@@ -6282,7 +6265,7 @@
         <v>255</v>
       </c>
       <c r="K191" s="7" t="s">
-        <v>363</v>
+        <v>347</v>
       </c>
       <c r="L191" s="7"/>
     </row>
@@ -6306,7 +6289,7 @@
         <v>255</v>
       </c>
       <c r="K192" s="7" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="L192" s="7"/>
     </row>
@@ -6341,13 +6324,13 @@
       </c>
       <c r="F194" s="3"/>
       <c r="I194" s="24" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="J194" s="12" t="s">
         <v>255</v>
       </c>
       <c r="K194" s="7" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
       <c r="L194" s="7"/>
     </row>
@@ -6370,10 +6353,10 @@
         <v>125</v>
       </c>
       <c r="J195" s="12" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="K195" s="7" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="L195" s="7"/>
     </row>
@@ -6393,7 +6376,7 @@
       <c r="I196" s="18"/>
       <c r="J196" s="18"/>
       <c r="K196" s="7" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
       <c r="L196" s="7"/>
     </row>
@@ -6414,10 +6397,10 @@
         <v>184</v>
       </c>
       <c r="J197" s="12" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="K197" s="7" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
       <c r="L197" s="7"/>
     </row>
@@ -6442,7 +6425,7 @@
         <v>255</v>
       </c>
       <c r="K198" s="7" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="L198" s="7"/>
     </row>
@@ -6459,7 +6442,7 @@
       </c>
       <c r="F199" s="3"/>
       <c r="K199" s="7" t="s">
-        <v>409</v>
+        <v>392</v>
       </c>
       <c r="L199" s="7"/>
     </row>
@@ -6473,7 +6456,7 @@
         <v>262</v>
       </c>
       <c r="K200" s="7" t="s">
-        <v>410</v>
+        <v>393</v>
       </c>
       <c r="L200" s="7"/>
     </row>
@@ -6496,7 +6479,7 @@
         <v>264</v>
       </c>
       <c r="K201" s="7" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="L201" s="7"/>
     </row>
@@ -6515,13 +6498,13 @@
         <v>24</v>
       </c>
       <c r="I202" s="24" t="s">
-        <v>417</v>
+        <v>399</v>
       </c>
       <c r="J202" s="12" t="s">
         <v>255</v>
       </c>
       <c r="K202" s="7" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
       <c r="L202" s="7"/>
     </row>
@@ -6554,13 +6537,13 @@
       </c>
       <c r="F204" s="3"/>
       <c r="I204" s="24" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="J204" s="12" t="s">
         <v>255</v>
       </c>
       <c r="K204" s="7" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
       <c r="L204" s="7"/>
     </row>
@@ -6583,10 +6566,10 @@
         <v>125</v>
       </c>
       <c r="J205" s="12" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="K205" s="7" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
       <c r="L205" s="7"/>
     </row>
@@ -6606,7 +6589,7 @@
       <c r="I206" s="18"/>
       <c r="J206" s="18"/>
       <c r="K206" s="7" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="L206" s="7"/>
     </row>
@@ -6627,10 +6610,10 @@
         <v>184</v>
       </c>
       <c r="J207" s="12" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="K207" s="7" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="L207" s="7"/>
     </row>
@@ -6655,7 +6638,7 @@
         <v>255</v>
       </c>
       <c r="K208" s="7" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="L208" s="7"/>
     </row>
@@ -6672,7 +6655,7 @@
       </c>
       <c r="F209" s="3"/>
       <c r="K209" s="7" t="s">
-        <v>411</v>
+        <v>394</v>
       </c>
       <c r="L209" s="7"/>
     </row>
@@ -6686,7 +6669,7 @@
         <v>262</v>
       </c>
       <c r="K210" s="7" t="s">
-        <v>412</v>
+        <v>395</v>
       </c>
       <c r="L210" s="7"/>
     </row>
@@ -6709,7 +6692,7 @@
         <v>264</v>
       </c>
       <c r="K211" s="7" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="L211" s="7"/>
     </row>
@@ -6728,13 +6711,13 @@
         <v>24</v>
       </c>
       <c r="I212" s="24" t="s">
-        <v>417</v>
+        <v>399</v>
       </c>
       <c r="J212" s="12" t="s">
         <v>255</v>
       </c>
       <c r="K212" s="7" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="L212" s="7"/>
     </row>
@@ -6790,10 +6773,10 @@
         <v>153</v>
       </c>
       <c r="J215" s="17" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="K215" s="7" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="L215" s="7"/>
     </row>
@@ -6813,13 +6796,13 @@
         <v>44</v>
       </c>
       <c r="I216" s="25" t="s">
-        <v>415</v>
+        <v>397</v>
       </c>
       <c r="J216" s="17" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="K216" s="7" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="L216" s="7"/>
     </row>
@@ -6839,7 +6822,7 @@
       <c r="I217" s="17"/>
       <c r="J217" s="17"/>
       <c r="K217" s="7" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="L217" s="7"/>
     </row>
@@ -6860,10 +6843,10 @@
         <v>154</v>
       </c>
       <c r="J218" s="13" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="K218" s="7" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="L218" s="7"/>
     </row>
@@ -6887,7 +6870,7 @@
         <v>255</v>
       </c>
       <c r="K219" s="7" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="L219" s="7"/>
     </row>
@@ -6911,7 +6894,7 @@
         <v>255</v>
       </c>
       <c r="K220" s="7" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="L220" s="7"/>
     </row>
@@ -6935,7 +6918,7 @@
         <v>255</v>
       </c>
       <c r="K221" s="7" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="L221" s="7"/>
     </row>
@@ -6959,7 +6942,7 @@
         <v>255</v>
       </c>
       <c r="K222" s="7" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="L222" s="7"/>
     </row>
@@ -6983,7 +6966,7 @@
         <v>255</v>
       </c>
       <c r="K223" s="7" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="L223" s="7"/>
     </row>
@@ -7007,7 +6990,7 @@
         <v>255</v>
       </c>
       <c r="K224" s="7" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
       <c r="L224" s="7"/>
     </row>
@@ -7048,7 +7031,7 @@
         <v>255</v>
       </c>
       <c r="K226" s="7" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
       <c r="L226" s="7"/>
     </row>
@@ -7099,13 +7082,13 @@
         <v>59</v>
       </c>
       <c r="I229" s="24" t="s">
-        <v>418</v>
+        <v>400</v>
       </c>
       <c r="J229" s="12" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="K229" s="7" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
       <c r="L229" s="7"/>
     </row>
@@ -7126,10 +7109,10 @@
         <v>222</v>
       </c>
       <c r="J230" s="13" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="K230" s="7" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
       <c r="L230" s="7"/>
     </row>
@@ -7147,13 +7130,13 @@
       </c>
       <c r="F231" s="3"/>
       <c r="I231" s="22" t="s">
-        <v>420</v>
+        <v>402</v>
       </c>
       <c r="J231" s="16" t="s">
         <v>255</v>
       </c>
       <c r="K231" s="7" t="s">
-        <v>393</v>
+        <v>377</v>
       </c>
       <c r="L231" s="7"/>
     </row>
@@ -7177,7 +7160,7 @@
         <v>255</v>
       </c>
       <c r="K232" s="7" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
       <c r="L232" s="7"/>
     </row>
@@ -7195,13 +7178,13 @@
       </c>
       <c r="F233" s="3"/>
       <c r="I233" s="26" t="s">
-        <v>419</v>
+        <v>401</v>
       </c>
       <c r="J233" s="13" t="s">
         <v>255</v>
       </c>
       <c r="K233" s="7" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
       <c r="L233" s="7"/>
     </row>
@@ -7225,7 +7208,7 @@
         <v>255</v>
       </c>
       <c r="K234" s="7" t="s">
-        <v>396</v>
+        <v>380</v>
       </c>
       <c r="L234" s="7"/>
     </row>
@@ -7249,7 +7232,7 @@
         <v>255</v>
       </c>
       <c r="K235" s="7" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="L235" s="7"/>
     </row>
@@ -7273,7 +7256,7 @@
         <v>255</v>
       </c>
       <c r="K236" s="7" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="L236" s="7"/>
     </row>
@@ -7300,7 +7283,7 @@
       </c>
       <c r="J237" s="12"/>
       <c r="K237" s="7" t="s">
-        <v>399</v>
+        <v>383</v>
       </c>
       <c r="L237" s="7"/>
     </row>

</xml_diff>